<commit_message>
Added DS18S20 and DS1822 sensors support
</commit_message>
<xml_diff>
--- a/sensors/Sensors.xlsx
+++ b/sensors/Sensors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quenon\Desktop\unleashed-firmware\applications\plugins\unitemp\sensors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{997A9972-1CE3-41BF-B045-01E70A5498EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF64809-A2CB-459A-B87C-8A6116BAD6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24761252-9F86-4A6F-8BB6-52E17BE4300A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
   <si>
     <t>Temperature</t>
   </si>
@@ -174,6 +174,115 @@
     <t>2.7 - 5.5 V</t>
   </si>
   <si>
+    <t>20 - 95 %</t>
+  </si>
+  <si>
+    <t>0.1 %</t>
+  </si>
+  <si>
+    <t>2.2 - 5.5 V</t>
+  </si>
+  <si>
+    <t>I2C</t>
+  </si>
+  <si>
+    <t>-40 - 80 °C</t>
+  </si>
+  <si>
+    <t>0 - 100%</t>
+  </si>
+  <si>
+    <t>DHT21 (AM2301)</t>
+  </si>
+  <si>
+    <t>DHT20 (AM2108)</t>
+  </si>
+  <si>
+    <t>3.3 - 5.2 V</t>
+  </si>
+  <si>
+    <t>DHT22 (AM2302)</t>
+  </si>
+  <si>
+    <t>AM2320</t>
+  </si>
+  <si>
+    <t>Single wire</t>
+  </si>
+  <si>
+    <t>Single wire, I2C</t>
+  </si>
+  <si>
+    <t>3.1 - 5.5 V</t>
+  </si>
+  <si>
+    <t>LM75</t>
+  </si>
+  <si>
+    <t>-55 - 125°C</t>
+  </si>
+  <si>
+    <t>0.5 °C</t>
+  </si>
+  <si>
+    <t>3 - 5.5 V</t>
+  </si>
+  <si>
+    <t>DS18B20</t>
+  </si>
+  <si>
+    <t>One Wire</t>
+  </si>
+  <si>
+    <t>DS1822</t>
+  </si>
+  <si>
+    <t>DS18S20 (DS1820)</t>
+  </si>
+  <si>
+    <t>BMP280</t>
+  </si>
+  <si>
+    <t>-40 - 85 °C</t>
+  </si>
+  <si>
+    <t>300-1100 hPA</t>
+  </si>
+  <si>
+    <t>1.71 - 3.6 V</t>
+  </si>
+  <si>
+    <r>
+      <t>I2C,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> SPI</t>
+    </r>
+  </si>
+  <si>
+    <t>±1.0 hPa</t>
+  </si>
+  <si>
+    <t>±3 %</t>
+  </si>
+  <si>
+    <t>±2%</t>
+  </si>
+  <si>
+    <t>±3%</t>
+  </si>
+  <si>
+    <t>0.0016 hPa</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -182,7 +291,7 @@
         <family val="2"/>
         <charset val="204"/>
       </rPr>
-      <t xml:space="preserve">0.5 ± </t>
+      <t xml:space="preserve"> ±0.5 </t>
     </r>
     <r>
       <rPr>
@@ -197,74 +306,63 @@
     </r>
   </si>
   <si>
-    <t>20 - 95 %</t>
-  </si>
-  <si>
-    <t>5 ± %</t>
-  </si>
-  <si>
-    <t>0.1 %</t>
-  </si>
-  <si>
-    <t>2.2 - 5.5 V</t>
-  </si>
-  <si>
-    <t>I2C</t>
-  </si>
-  <si>
-    <t>-40 - 80 °C</t>
-  </si>
-  <si>
-    <t>0 - 100%</t>
-  </si>
-  <si>
-    <t>3 ± %</t>
-  </si>
-  <si>
-    <t>DHT21 (AM2301)</t>
-  </si>
-  <si>
-    <t>DHT20 (AM2108)</t>
-  </si>
-  <si>
-    <t>3.3 - 5.2 V</t>
-  </si>
-  <si>
-    <t>DHT22 (AM2302)</t>
-  </si>
-  <si>
-    <t>2 ± %</t>
-  </si>
-  <si>
-    <t>AM2320</t>
-  </si>
-  <si>
-    <t>Single wire</t>
-  </si>
-  <si>
-    <t>Single wire, I2C</t>
-  </si>
-  <si>
-    <t>3.1 - 5.5 V</t>
-  </si>
-  <si>
-    <t>LM75</t>
-  </si>
-  <si>
-    <t>-55 - 125°C</t>
-  </si>
-  <si>
-    <t>0.5 °C</t>
-  </si>
-  <si>
-    <t>3 - 5.5 V</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> ±0.5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> ±0.5 °C</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve">±0.5 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <t>0.01 °C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -298,6 +396,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -352,21 +458,22 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% — акцент3" xfId="2" builtinId="40"/>
@@ -683,10 +790,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30197D5-1B8F-46B2-AB75-05B6E656A3AB}">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,340 +805,450 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="E10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
+      <c r="F10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="E12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E15" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="G15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H15" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I15" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Added sensor analogues names
</commit_message>
<xml_diff>
--- a/sensors/Sensors.xlsx
+++ b/sensors/Sensors.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quenon\Desktop\unleashed-firmware\applications\plugins\unitemp\sensors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quenon\Desktop\flipperzero-firmware\applications\plugins\unitemp\sensors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF64809-A2CB-459A-B87C-8A6116BAD6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A254F0-7817-44AC-9C4E-11C820012341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24761252-9F86-4A6F-8BB6-52E17BE4300A}"/>
   </bookViews>
@@ -210,9 +210,6 @@
     <t>Single wire</t>
   </si>
   <si>
-    <t>Single wire, I2C</t>
-  </si>
-  <si>
     <t>3.1 - 5.5 V</t>
   </si>
   <si>
@@ -356,6 +353,22 @@
   </si>
   <si>
     <t>0.01 °C</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Single wire, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>I2C</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -467,13 +480,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="60% — акцент3" xfId="2" builtinId="40"/>
@@ -793,7 +806,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -805,35 +818,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6" t="s">
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="7"/>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
@@ -934,13 +947,13 @@
         <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>18</v>
@@ -972,7 +985,7 @@
         <v>33</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
@@ -981,7 +994,7 @@
         <v>34</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>15</v>
@@ -1004,7 +1017,7 @@
         <v>33</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>18</v>
@@ -1013,7 +1026,7 @@
         <v>34</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>30</v>
@@ -1027,16 +1040,16 @@
         <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>18</v>
@@ -1045,7 +1058,7 @@
         <v>34</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>30</v>
@@ -1061,25 +1074,25 @@
       <c r="B9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" s="8" t="s">
+      <c r="H9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>30</v>
       </c>
       <c r="J9" s="4"/>
@@ -1088,22 +1101,22 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -1114,51 +1127,51 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>52</v>
-      </c>
       <c r="E11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>18</v>
@@ -1172,22 +1185,22 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -1198,16 +1211,16 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Added support for AM2320 sensor by I2C. Optimized work with I2C
</commit_message>
<xml_diff>
--- a/sensors/Sensors.xlsx
+++ b/sensors/Sensors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quenon\Desktop\flipperzero-firmware\applications\plugins\unitemp\sensors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A254F0-7817-44AC-9C4E-11C820012341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007D04C4-208D-45A4-8F57-0D04FB2B9A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24761252-9F86-4A6F-8BB6-52E17BE4300A}"/>
+    <workbookView xWindow="3585" yWindow="3510" windowWidth="21525" windowHeight="11385" xr2:uid="{24761252-9F86-4A6F-8BB6-52E17BE4300A}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="67">
   <si>
     <t>Temperature</t>
   </si>
@@ -198,9 +198,6 @@
     <t>DHT20 (AM2108)</t>
   </si>
   <si>
-    <t>3.3 - 5.2 V</t>
-  </si>
-  <si>
     <t>DHT22 (AM2302)</t>
   </si>
   <si>
@@ -247,22 +244,6 @@
   </si>
   <si>
     <t>1.71 - 3.6 V</t>
-  </si>
-  <si>
-    <r>
-      <t>I2C,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> SPI</t>
-    </r>
   </si>
   <si>
     <t>±1.0 hPa</t>
@@ -355,27 +336,43 @@
     <t>0.01 °C</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Single wire, </t>
-    </r>
+    <t>2.8 - 5.5 V</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> ±1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>I2C</t>
-    </r>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <t>3.3 - 5 V</t>
+  </si>
+  <si>
+    <t>Single wire, I2C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,14 +406,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -806,7 +795,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +872,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>17</v>
@@ -915,7 +904,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>16</v>
@@ -947,13 +936,13 @@
         <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>65</v>
+        <v>39</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>18</v>
@@ -976,16 +965,16 @@
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>18</v>
@@ -994,10 +983,10 @@
         <v>34</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
@@ -1005,19 +994,19 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>18</v>
@@ -1026,7 +1015,7 @@
         <v>34</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>30</v>
@@ -1037,19 +1026,19 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>18</v>
@@ -1058,7 +1047,7 @@
         <v>34</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>30</v>
@@ -1081,7 +1070,7 @@
         <v>33</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>18</v>
@@ -1090,7 +1079,7 @@
         <v>34</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I9" s="6" t="s">
         <v>30</v>
@@ -1101,22 +1090,22 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -1127,51 +1116,51 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>51</v>
-      </c>
       <c r="E11" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>18</v>
@@ -1185,22 +1174,22 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -1211,16 +1200,16 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Added new sensors SHT30/31/35, GXHT30/31/35
</commit_message>
<xml_diff>
--- a/sensors/Sensors.xlsx
+++ b/sensors/Sensors.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quenon\Desktop\flipperzero-firmware\applications\plugins\unitemp\sensors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Quenon\Desktop\unleashed-firmware\applications\plugins\unitemp_flipperzero\sensors\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4176AB82-BE29-46F0-84FC-BC6E32C866D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97AA3276-7F2D-47DB-8760-8FA46B76DC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24761252-9F86-4A6F-8BB6-52E17BE4300A}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{24761252-9F86-4A6F-8BB6-52E17BE4300A}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="78">
   <si>
     <t>Temperature</t>
   </si>
@@ -360,6 +360,73 @@
   </si>
   <si>
     <t>2…5.5V</t>
+  </si>
+  <si>
+    <t>SHT30/GXHT30</t>
+  </si>
+  <si>
+    <t>2.2…5.5V</t>
+  </si>
+  <si>
+    <t>0.06 °C</t>
+  </si>
+  <si>
+    <t>±1.5%</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> ±0.1 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <t>SHT31/GXHT31</t>
+  </si>
+  <si>
+    <t>SHT35/GXHT35</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> ±0.2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>°C</t>
+    </r>
+  </si>
+  <si>
+    <t>-40…125 °C</t>
   </si>
 </sst>
 </file>
@@ -448,14 +515,14 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -772,10 +839,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30197D5-1B8F-46B2-AB75-05B6E656A3AB}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L17"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -794,35 +861,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5" t="s">
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="5"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1012,7 +1079,7 @@
       <c r="L7" s="4"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>66</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -1141,115 +1208,115 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>69</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>47</v>
+        <v>77</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>9</v>
+        <v>64</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+        <v>71</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>75</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>35</v>
+        <v>73</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>46</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="L14" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>32</v>
+        <v>9</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>13</v>
@@ -1263,55 +1330,151 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
+      <c r="J16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>